<commit_message>
Fixes documentation in code and sprint
Adds doc strings, wireframe, class diagram, and adds more to sprint backlog
</commit_message>
<xml_diff>
--- a/sprints/sprint4/Group 4 Sprint 4 Sprint Backlog.xlsx
+++ b/sprints/sprint4/Group 4 Sprint 4 Sprint Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavincoppola/workspace/Capstone2024Group4/sprints/sprint4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0C1228-9414-C14A-9AFC-89ED6CB90359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BC52F4-7E61-0E4B-BCEA-D48F10782A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -78,6 +78,21 @@
   <si>
     <t>4 hours</t>
   </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>Address Noted Concerns</t>
+  </si>
+  <si>
+    <t>Fix web page reponsive issues</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>Add cancel to editing notes</t>
+  </si>
 </sst>
 </file>
 
@@ -95,11 +110,13 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -386,7 +403,7 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -532,8 +549,12 @@
       <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -569,8 +590,12 @@
       <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -606,8 +631,12 @@
       <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -644,7 +673,9 @@
         <v>6</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -668,11 +699,22 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="4"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -696,11 +738,22 @@
       <c r="AA8" s="2"/>
     </row>
     <row r="9" spans="1:27" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>

</xml_diff>